<commit_message>
add lab notebook page template. updated mcal tbls.
</commit_message>
<xml_diff>
--- a/mp_eval_tbls_template.xlsx
+++ b/mp_eval_tbls_template.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/OMNIBUS/riveraomics/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/OMNIBUS/riveraomics/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{885FEB90-CF40-DA43-9427-D73F05B73376}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36E2EBEB-E0B2-DC42-896A-EADC49932F87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="21600" windowHeight="33300" xr2:uid="{E26EA2C6-5320-404E-A7C5-C961A940C7FB}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="31220" windowHeight="22540" xr2:uid="{E26EA2C6-5320-404E-A7C5-C961A940C7FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -145,7 +145,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -182,6 +182,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE2EFDB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="25">
     <border>
@@ -471,14 +477,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -496,8 +502,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -532,7 +536,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -542,9 +545,6 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -563,44 +563,62 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -610,6 +628,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFE2EFDB"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -920,8 +943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B47C03FC-16A5-1D4E-BE75-E7AF4A81EDB1}">
   <dimension ref="B1:I55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="157" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="157" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -941,17 +964,17 @@
     </row>
     <row r="2" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B3" s="47" t="s">
+      <c r="B3" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="49"/>
-      <c r="I3" s="45"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="39"/>
+      <c r="I3" s="36"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="15" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="13" t="s">
@@ -963,102 +986,102 @@
       <c r="E4" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="18" t="s">
+      <c r="F4" s="16" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B5" s="30">
+      <c r="B5" s="27">
         <v>1</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
       <c r="E5" s="10"/>
-      <c r="F5" s="19"/>
+      <c r="F5" s="17"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B6" s="31">
+      <c r="B6" s="28">
         <v>2</v>
       </c>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
       <c r="E6" s="10"/>
-      <c r="F6" s="20"/>
+      <c r="F6" s="18"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B7" s="31">
+      <c r="B7" s="28">
         <v>3</v>
       </c>
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
       <c r="E7" s="10"/>
-      <c r="F7" s="21"/>
+      <c r="F7" s="19"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B8" s="31">
+      <c r="B8" s="28">
         <v>4</v>
       </c>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
       <c r="E8" s="10"/>
-      <c r="F8" s="21"/>
+      <c r="F8" s="19"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B9" s="31">
+      <c r="B9" s="28">
         <v>5</v>
       </c>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
       <c r="E9" s="10"/>
-      <c r="F9" s="21"/>
+      <c r="F9" s="19"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B10" s="31">
+      <c r="B10" s="28">
         <v>6</v>
       </c>
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
       <c r="E10" s="10"/>
-      <c r="F10" s="21"/>
+      <c r="F10" s="19"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B11" s="31">
+      <c r="B11" s="28">
         <v>7</v>
       </c>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
       <c r="E11" s="10"/>
-      <c r="F11" s="21"/>
+      <c r="F11" s="19"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B12" s="31">
+      <c r="B12" s="28">
         <v>8</v>
       </c>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
       <c r="E12" s="10"/>
-      <c r="F12" s="21"/>
+      <c r="F12" s="19"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B13" s="31">
+      <c r="B13" s="28">
         <v>9</v>
       </c>
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
       <c r="E13" s="10"/>
-      <c r="F13" s="21"/>
+      <c r="F13" s="19"/>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B14" s="32">
+      <c r="B14" s="29">
         <v>10</v>
       </c>
       <c r="C14" s="11"/>
       <c r="D14" s="11"/>
       <c r="E14" s="12"/>
-      <c r="F14" s="21"/>
+      <c r="F14" s="19"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B15" s="36" t="s">
+      <c r="B15" s="30" t="s">
         <v>1</v>
       </c>
       <c r="C15" s="5">
@@ -1073,10 +1096,10 @@
         <f t="shared" ref="E15" si="1">MIN(E5:E14)</f>
         <v>0</v>
       </c>
-      <c r="F15" s="21"/>
+      <c r="F15" s="19"/>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B16" s="37" t="s">
+      <c r="B16" s="31" t="s">
         <v>2</v>
       </c>
       <c r="C16" s="2">
@@ -1091,10 +1114,10 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F16" s="21"/>
+      <c r="F16" s="19"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B17" s="37" t="s">
+      <c r="B17" s="31" t="s">
         <v>3</v>
       </c>
       <c r="C17" s="2" t="e">
@@ -1109,10 +1132,10 @@
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="F17" s="21"/>
+      <c r="F17" s="19"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B18" s="37" t="s">
+      <c r="B18" s="31" t="s">
         <v>4</v>
       </c>
       <c r="C18" s="2" t="e">
@@ -1127,10 +1150,10 @@
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="F18" s="21"/>
+      <c r="F18" s="19"/>
     </row>
     <row r="19" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="38" t="s">
+      <c r="B19" s="32" t="s">
         <v>5</v>
       </c>
       <c r="C19" s="4" t="e">
@@ -1141,24 +1164,24 @@
         <f t="shared" ref="D19" si="5">(D18/D17)*100</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E19" s="22" t="e">
+      <c r="E19" s="20" t="e">
         <f t="shared" ref="E19" si="6">(E18/E17)*100</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F19" s="23"/>
+      <c r="F19" s="21"/>
     </row>
     <row r="20" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="21" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B21" s="50" t="s">
+      <c r="B21" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="51"/>
-      <c r="D21" s="51"/>
-      <c r="E21" s="51"/>
-      <c r="F21" s="52"/>
+      <c r="C21" s="41"/>
+      <c r="D21" s="41"/>
+      <c r="E21" s="41"/>
+      <c r="F21" s="42"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B22" s="24" t="s">
+      <c r="B22" s="22" t="s">
         <v>7</v>
       </c>
       <c r="C22" s="13" t="s">
@@ -1170,102 +1193,102 @@
       <c r="E22" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="F22" s="25" t="s">
+      <c r="F22" s="23" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B23" s="30">
+      <c r="B23" s="27">
         <v>1</v>
       </c>
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
       <c r="E23" s="9"/>
-      <c r="F23" s="26"/>
+      <c r="F23" s="24"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B24" s="31">
+      <c r="B24" s="28">
         <v>2</v>
       </c>
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
       <c r="E24" s="9"/>
-      <c r="F24" s="27"/>
+      <c r="F24" s="25"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B25" s="31">
+      <c r="B25" s="28">
         <v>3</v>
       </c>
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
       <c r="E25" s="9"/>
-      <c r="F25" s="28"/>
+      <c r="F25" s="26"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B26" s="31">
+      <c r="B26" s="28">
         <v>4</v>
       </c>
       <c r="C26" s="9"/>
       <c r="D26" s="9"/>
       <c r="E26" s="9"/>
-      <c r="F26" s="28"/>
+      <c r="F26" s="26"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B27" s="31">
+      <c r="B27" s="28">
         <v>5</v>
       </c>
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
       <c r="E27" s="9"/>
-      <c r="F27" s="28"/>
+      <c r="F27" s="26"/>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B28" s="31">
+      <c r="B28" s="28">
         <v>6</v>
       </c>
       <c r="C28" s="9"/>
       <c r="D28" s="9"/>
       <c r="E28" s="9"/>
-      <c r="F28" s="28"/>
+      <c r="F28" s="26"/>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B29" s="31">
+      <c r="B29" s="28">
         <v>7</v>
       </c>
       <c r="C29" s="9"/>
       <c r="D29" s="9"/>
       <c r="E29" s="9"/>
-      <c r="F29" s="28"/>
+      <c r="F29" s="26"/>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B30" s="31">
+      <c r="B30" s="28">
         <v>8</v>
       </c>
       <c r="C30" s="9"/>
       <c r="D30" s="9"/>
       <c r="E30" s="9"/>
-      <c r="F30" s="28"/>
+      <c r="F30" s="26"/>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B31" s="31">
+      <c r="B31" s="28">
         <v>9</v>
       </c>
       <c r="C31" s="9"/>
       <c r="D31" s="9"/>
       <c r="E31" s="9"/>
-      <c r="F31" s="28"/>
+      <c r="F31" s="26"/>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B32" s="32">
+      <c r="B32" s="29">
         <v>10</v>
       </c>
       <c r="C32" s="11"/>
       <c r="D32" s="11"/>
       <c r="E32" s="11"/>
-      <c r="F32" s="28"/>
+      <c r="F32" s="26"/>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B33" s="39" t="s">
+      <c r="B33" s="33" t="s">
         <v>1</v>
       </c>
       <c r="C33" s="5">
@@ -1280,10 +1303,10 @@
         <f t="shared" ref="E33" si="8">MIN(E23:E32)</f>
         <v>0</v>
       </c>
-      <c r="F33" s="21"/>
+      <c r="F33" s="19"/>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B34" s="40" t="s">
+      <c r="B34" s="34" t="s">
         <v>2</v>
       </c>
       <c r="C34" s="2">
@@ -1298,10 +1321,10 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="F34" s="21"/>
+      <c r="F34" s="19"/>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B35" s="40" t="s">
+      <c r="B35" s="34" t="s">
         <v>3</v>
       </c>
       <c r="C35" s="2" t="e">
@@ -1316,10 +1339,10 @@
         <f t="shared" si="10"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="F35" s="21"/>
+      <c r="F35" s="19"/>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B36" s="40" t="s">
+      <c r="B36" s="34" t="s">
         <v>4</v>
       </c>
       <c r="C36" s="2" t="e">
@@ -1334,10 +1357,10 @@
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="F36" s="21"/>
+      <c r="F36" s="19"/>
     </row>
     <row r="37" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="41" t="s">
+      <c r="B37" s="35" t="s">
         <v>5</v>
       </c>
       <c r="C37" s="4" t="e">
@@ -1348,131 +1371,131 @@
         <f t="shared" ref="D37" si="12">(D36/D35)*100</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E37" s="22" t="e">
+      <c r="E37" s="20" t="e">
         <f>(E36/E35)*100</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F37" s="23"/>
+      <c r="F37" s="21"/>
     </row>
     <row r="38" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="39" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B39" s="53" t="s">
+      <c r="B39" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="C39" s="54"/>
-      <c r="D39" s="54"/>
-      <c r="E39" s="54"/>
-      <c r="F39" s="55"/>
+      <c r="C39" s="44"/>
+      <c r="D39" s="44"/>
+      <c r="E39" s="44"/>
+      <c r="F39" s="45"/>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B40" s="29" t="s">
+      <c r="B40" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="C40" s="15" t="s">
+      <c r="C40" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="D40" s="15" t="s">
+      <c r="D40" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="E40" s="16" t="s">
+      <c r="E40" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="F40" s="18" t="s">
+      <c r="F40" s="16" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B41" s="33">
+      <c r="B41" s="47">
         <v>1</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
       <c r="E41" s="7"/>
-      <c r="F41" s="19"/>
+      <c r="F41" s="17"/>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B42" s="34">
+      <c r="B42" s="48">
         <v>2</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
       <c r="E42" s="7"/>
-      <c r="F42" s="20"/>
+      <c r="F42" s="18"/>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B43" s="34">
+      <c r="B43" s="48">
         <v>3</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
       <c r="E43" s="7"/>
-      <c r="F43" s="21"/>
+      <c r="F43" s="19"/>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B44" s="34">
+      <c r="B44" s="48">
         <v>4</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
       <c r="E44" s="7"/>
-      <c r="F44" s="21"/>
+      <c r="F44" s="19"/>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B45" s="34">
+      <c r="B45" s="48">
         <v>5</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
       <c r="E45" s="7"/>
-      <c r="F45" s="21"/>
+      <c r="F45" s="19"/>
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B46" s="34">
+      <c r="B46" s="48">
         <v>6</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
       <c r="E46" s="7"/>
-      <c r="F46" s="21"/>
+      <c r="F46" s="19"/>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B47" s="34">
+      <c r="B47" s="48">
         <v>7</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
       <c r="E47" s="7"/>
-      <c r="F47" s="21"/>
+      <c r="F47" s="19"/>
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B48" s="34">
+      <c r="B48" s="48">
         <v>8</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
       <c r="E48" s="7"/>
-      <c r="F48" s="21"/>
+      <c r="F48" s="19"/>
     </row>
     <row r="49" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B49" s="34">
+      <c r="B49" s="48">
         <v>9</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
       <c r="E49" s="7"/>
-      <c r="F49" s="21"/>
+      <c r="F49" s="19"/>
     </row>
     <row r="50" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B50" s="35">
+      <c r="B50" s="49">
         <v>10</v>
       </c>
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
       <c r="E50" s="8"/>
-      <c r="F50" s="21"/>
+      <c r="F50" s="19"/>
     </row>
     <row r="51" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B51" s="42" t="s">
+      <c r="B51" s="50" t="s">
         <v>1</v>
       </c>
       <c r="C51" s="5">
@@ -1487,10 +1510,10 @@
         <f>MIN(E41:E50)</f>
         <v>0</v>
       </c>
-      <c r="F51" s="21"/>
+      <c r="F51" s="19"/>
     </row>
     <row r="52" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B52" s="43" t="s">
+      <c r="B52" s="51" t="s">
         <v>2</v>
       </c>
       <c r="C52" s="2">
@@ -1505,10 +1528,10 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="F52" s="21"/>
+      <c r="F52" s="19"/>
     </row>
     <row r="53" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B53" s="43" t="s">
+      <c r="B53" s="51" t="s">
         <v>3</v>
       </c>
       <c r="C53" s="2" t="e">
@@ -1523,10 +1546,10 @@
         <f t="shared" si="15"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="F53" s="21"/>
+      <c r="F53" s="19"/>
     </row>
     <row r="54" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B54" s="43" t="s">
+      <c r="B54" s="51" t="s">
         <v>4</v>
       </c>
       <c r="C54" s="2" t="e">
@@ -1541,10 +1564,10 @@
         <f>STDEV(E41:E50)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F54" s="21"/>
+      <c r="F54" s="19"/>
     </row>
     <row r="55" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="44" t="s">
+      <c r="B55" s="52" t="s">
         <v>5</v>
       </c>
       <c r="C55" s="4" t="e">
@@ -1555,11 +1578,11 @@
         <f t="shared" ref="D55" si="17">(D54/D53)*100</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E55" s="22" t="e">
+      <c r="E55" s="20" t="e">
         <f>(E54/E53)*100</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F55" s="23"/>
+      <c r="F55" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1569,5 +1592,6 @@
     <mergeCell ref="B1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>